<commit_message>
lr update sch sth form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_1_school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Liberia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C1D85D-5252-48E2-A331-FDB94D09581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E43FF2-FC0F-4EE8-BC7E-10FBA436B2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>type</t>
   </si>
@@ -154,9 +154,6 @@
     <t>The two digit code assigned to you</t>
   </si>
   <si>
-    <t>lr_sch_sth_impact_202401_1_school</t>
-  </si>
-  <si>
     <t>w_school_name</t>
   </si>
   <si>
@@ -244,13 +241,22 @@
     <t>w_school_community</t>
   </si>
   <si>
-    <t>(2024 Jan) - 1. SCH/STH – Site Level (School or Community) Form</t>
-  </si>
-  <si>
     <t>w_school_id</t>
   </si>
   <si>
     <t>w_sub_district</t>
+  </si>
+  <si>
+    <t>. &gt; 99 and . &lt; 1000</t>
+  </si>
+  <si>
+    <t>Must be two digit between 99 and 1000</t>
+  </si>
+  <si>
+    <t>(2024 Jan) - 1. SCH/STH – Site Level (School or Community) Form V1.2</t>
+  </si>
+  <si>
+    <t>lr_sch_sth_impact_202401_1_school_v1_2</t>
   </si>
 </sst>
 </file>
@@ -779,11 +785,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -841,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -904,7 +910,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="11"/>
@@ -924,10 +930,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="11"/>
@@ -947,10 +953,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="11"/>
@@ -965,20 +971,24 @@
       <c r="L6" s="17"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
@@ -993,10 +1003,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="11"/>
@@ -1019,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>36</v>
@@ -1041,10 +1051,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="11"/>
@@ -1064,10 +1074,10 @@
         <v>29</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="11"/>
@@ -1084,13 +1094,13 @@
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="11"/>
@@ -1110,10 +1120,10 @@
         <v>29</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="11"/>
@@ -1133,10 +1143,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="11"/>
@@ -1156,10 +1166,10 @@
         <v>29</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="11"/>
@@ -1268,7 +1278,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -1279,68 +1289,68 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1353,13 +1363,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="57.25" style="6" customWidth="1"/>
     <col min="2" max="2" width="36.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="15.875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="6"/>
@@ -1376,12 +1386,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
lr! update sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Liberia/lr_sch_sth_impact_202401_1_school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Liberia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6F27C-1C8C-4889-B8F2-6EFB6A2D6591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C9BFCB-BA18-4199-9705-62176230BA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1624,11 +1624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G186" sqref="G186"/>
     </sheetView>

</xml_diff>